<commit_message>
Ajuste do Processo para Trabalhar com a Planilha mais atualizada do CPS. Ajuste na convocação para desconsiderar ausentes. Ajuste para resolver problema de NPE não leitura de células vazias dos arquivos do tipo *.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/br/org/sae/test/arquivo-vazio.xlsx
+++ b/src/test/resources/br/org/sae/test/arquivo-vazio.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="dados" sheetId="1" r:id="rId1"/>
+    <sheet name="VESTIBULINHO" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>

</xml_diff>